<commit_message>
Code for Jsutify Exceptions
</commit_message>
<xml_diff>
--- a/Data/TestRun.xlsx
+++ b/Data/TestRun.xlsx
@@ -1,32 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8127A78-879F-445D-A771-1550A7FBB27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-876" yWindow="3204" windowWidth="16404" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
-    <sheet name="Full Time 40" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Full Time 40" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase">'Full Time 40'!$G$1:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase">'Full Time 40'!$F$1:$F$3</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
-  <si>
-    <t>EmpNum</t>
-  </si>
-  <si>
-    <t>ExpectedDescription</t>
-  </si>
-  <si>
-    <t>Date</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>EmpID</t>
+  </si>
+  <si>
+    <t>Paycodes</t>
   </si>
   <si>
     <t>FromDate</t>
@@ -41,7 +37,25 @@
     <t>TestResult</t>
   </si>
   <si>
-    <t>10510166</t>
+    <t>10649101</t>
+  </si>
+  <si>
+    <t>SK-Early Out Excused.,SK-Long Break Excused.,SK-Early Out Excused.</t>
+  </si>
+  <si>
+    <t>01/02/2025</t>
+  </si>
+  <si>
+    <t>28/02/2025</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>10510273</t>
   </si>
   <si>
     <t>less than the weekly minimum of 40 hours.</t>
@@ -51,12 +65,6 @@
   </si>
   <si>
     <t>09/03/2025</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>10510273</t>
   </si>
   <si>
     <t>Yes</t>
@@ -65,25 +73,25 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
+      <color indexed="8"/>
       <sz val="10"/>
-      <color indexed="8"/>
       <name val="Arial"/>
     </font>
     <font>
+      <color indexed="8"/>
+      <family val="2"/>
       <sz val="11"/>
-      <color indexed="8"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -106,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -118,9 +126,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -129,7 +135,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF009900"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -143,7 +149,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF009900"/>
         </patternFill>
       </fill>
     </dxf>
@@ -422,96 +428,93 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScale="120" zoomScaleNormal="120">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="111.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5546875" customWidth="1"/>
-    <col min="4" max="5" width="11.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="21.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5546875" customWidth="1"/>
+    <col min="3" max="4" width="11.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" ht="14.4" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" ht="14.4" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" ht="14.4" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>